<commit_message>
Added images for latex + corrected small error in xls
</commit_message>
<xml_diff>
--- a/6/evaluation.xlsx
+++ b/6/evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="895" firstSheet="9" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="895" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="push" sheetId="1" r:id="rId1"/>
@@ -5415,7 +5415,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-AT"/>
-              <a:t>Push &amp; Pull mit verschiedenen c Werten</a:t>
+              <a:t>Push &amp; Pull mit c=5</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11964,7 +11964,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -12060,7 +12060,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>